<commit_message>
Finishing first draft of chapter 3
</commit_message>
<xml_diff>
--- a/doc/theses/ellen_porter_mscs/drawings/DataDistribution.xlsx
+++ b/doc/theses/ellen_porter_mscs/drawings/DataDistribution.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\port091\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="7500" windowHeight="4950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29070" windowHeight="15870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -59,6 +64,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -70,10 +78,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="135"/>
+      <c14:style val="103"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="35"/>
+      <c:style val="3"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -87,6 +95,18 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="76000"/>
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
@@ -187,12 +207,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="0"/>
-        <c:axId val="38582528"/>
-        <c:axId val="40141568"/>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="187094352"/>
+        <c:axId val="187094912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38582528"/>
+        <c:axId val="187094352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -201,14 +222,24 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Voxel</a:t>
                 </a:r>
               </a:p>
@@ -216,11 +247,71 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40141568"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="187094912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -228,24 +319,48 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40141568"/>
+        <c:axId val="187094912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Triangle count</a:t>
                 </a:r>
               </a:p>
@@ -253,26 +368,1444 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="187094352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>399574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4383590</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1331300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45798</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2242646</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>228823</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1896809</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="189485776"/>
+        <c:axId val="189486336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="189485776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Node</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="189486336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="189486336"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Triangle Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38582528"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="189485776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -280,15 +1813,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -302,6 +1835,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -353,7 +1916,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +1951,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,87 +2160,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <f>SUM(B1:B9)</f>
+        <v>399574</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>399540</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>SUM(B10:B12)</f>
+        <v>4383590</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <f>SUM(B22:B24)</f>
+        <v>1331300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <f>SUM(B25:B27)</f>
+        <v>45798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f>SUM(B13:B15)</f>
+        <v>2242646</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f>SUM(B16:B18)</f>
+        <v>228823</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f>SUM(B19:B21)</f>
+        <v>1896809</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>SUM(D1:D8)</f>
+        <v>10528540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -685,7 +2307,7 @@
         <v>64723</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -693,7 +2315,7 @@
         <v>4318867</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -701,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -709,7 +2331,7 @@
         <v>15168</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -717,7 +2339,7 @@
         <v>2227478</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -725,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -819,6 +2441,12 @@
       </c>
       <c r="B27" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>SUM(B1:B27)</f>
+        <v>10528540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>